<commit_message>
Refix ZSS-852: Multiply array inside SUMPRODUCT is legal; out of SUMPRODUCT is relatively picking proper value in array; or #VALUE! if no way to pick that proper value.
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/issue/book/852-conditional-sumproduct.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/issue/book/852-conditional-sumproduct.xlsx
@@ -365,15 +365,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,12 +387,16 @@
         <f>SUMPRODUCT(--(A1:A3="John"),(B1:B3),(C1:C3))</f>
         <v>10</v>
       </c>
+      <c r="E1">
+        <f>SUMPRODUCT(F12:F21*H12:H21)</f>
+        <v>106</v>
+      </c>
       <c r="I1">
         <f>SUMPRODUCT((F12:F21=1)*(G12:G21="Z")*H12:H21)</f>
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -402,8 +406,28 @@
       <c r="C2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="D2">
+        <f>$B1:$B3+$C1:$C3</f>
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <f>$B1:$B3-$C1:$C3</f>
+        <v>-3</v>
+      </c>
+      <c r="F2">
+        <f>$B1:$B3*$C1:$C3</f>
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <f>$B1:$B3/$C1:$C3</f>
+        <v>0.4</v>
+      </c>
+      <c r="H2">
+        <f>POWER($B1:$B3, $C1:$C3)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -414,7 +438,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="7" spans="1:11">
+      <c r="K7" t="e">
+        <f>B1:B3*C1:C3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="F12">
         <v>1</v>
       </c>
@@ -425,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11">
       <c r="F13">
         <v>2</v>
       </c>
@@ -436,7 +466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:11">
       <c r="F14">
         <v>3</v>
       </c>
@@ -447,7 +477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11">
       <c r="F15">
         <v>1</v>
       </c>
@@ -458,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="F16">
         <v>2</v>
       </c>

</xml_diff>